<commit_message>
prayer modified on 1/4/2019
</commit_message>
<xml_diff>
--- a/prayers.xlsx
+++ b/prayers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bakytbek\Desktop\accounts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bakytbek\Desktop\soyuzbek\accounts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="B1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +679,7 @@
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <v>43327</v>
+        <v>43317</v>
       </c>
       <c r="C7" s="3">
         <v>20</v>
@@ -761,15 +761,30 @@
       <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <v>43469</v>
+      </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="E9" s="3">
+        <f>E8-3</f>
+        <v>149</v>
+      </c>
+      <c r="F9" s="3">
+        <v>530</v>
+      </c>
+      <c r="G9" s="3">
+        <v>560</v>
+      </c>
+      <c r="H9" s="3">
+        <v>560</v>
+      </c>
+      <c r="I9" s="3">
+        <v>575</v>
+      </c>
+      <c r="J9" s="3">
+        <v>2</v>
+      </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>

</xml_diff>